<commit_message>
changes in feature file to pass the test data for few test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/excelData.xlsx
+++ b/src/test/resources/excelData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>firstName</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Mani@123@#</t>
+  </si>
+  <si>
+    <t>Mani12**(</t>
   </si>
 </sst>
 </file>
@@ -398,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -468,6 +471,29 @@
         <v>9986981193</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>

</xml_diff>